<commit_message>
Use default column styles (fixes #317, see also #316)
</commit_message>
<xml_diff>
--- a/ExcelMapper.Tests/xlsx/dateformat.xlsx
+++ b/ExcelMapper.Tests/xlsx/dateformat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ExcelMapper\ExcelMapper.Tests\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\ExcelMapper\ExcelMapper.Tests\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE884A3-A306-4BDF-B902-D5ECDD8C72A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94A6DF9-5FB9-4292-9687-132325C47A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19992" windowHeight="12792" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -45,7 +45,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -54,14 +54,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF729FCF"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFA6"/>
-        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -77,10 +83,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -278,22 +285,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>45323</v>
       </c>
     </row>

</xml_diff>